<commit_message>
add monthly load visualization
</commit_message>
<xml_diff>
--- a/forecast_model/load model monthly calendar.xlsx
+++ b/forecast_model/load model monthly calendar.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dvsto\Documents\School Work\EBL Project\remote_hub_simulation\forecast_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3227224E-7B7A-4FA5-885F-57A91911B495}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D44ACE38-4485-4311-8A1B-67100BF5F6BA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5568" activeTab="1" xr2:uid="{2417AB51-40A1-449C-916A-28CDA729CCB4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5568" activeTab="2" xr2:uid="{2417AB51-40A1-449C-916A-28CDA729CCB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="13">
   <si>
     <t>low_on_peak</t>
   </si>
@@ -59,6 +60,18 @@
   </si>
   <si>
     <t>probability</t>
+  </si>
+  <si>
+    <t># of days (monthly)</t>
+  </si>
+  <si>
+    <t># of days (quarterly)</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>load_profile</t>
   </si>
 </sst>
 </file>
@@ -525,62 +538,430 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B024163-DA52-4784-9B0A-0C44648AF202}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.44140625" customWidth="1"/>
     <col min="2" max="2" width="10.44140625" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0.22</v>
+      </c>
+      <c r="C2">
+        <f>ROUND(B2*30,0)</f>
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <f>ROUND(B2*91.25,0)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0.27</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C8" si="0">ROUND(B3*30,0)</f>
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D8" si="1">ROUND(B3*91.25,0)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.19</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0.17</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0.1</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>0.04</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>0.01</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <f>SUM(B2:B8)</f>
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <f>SUM(C2:C8)</f>
+        <v>30</v>
+      </c>
+      <c r="D9">
+        <f>SUM(D2:D8)</f>
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09830079-3ED1-41B6-8A08-41DA39B99645}">
+  <dimension ref="A1:B31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>6</v>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B31">
+    <sortCondition ref="A2:A31"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>